<commit_message>
update PVS data xlsx
</commit_message>
<xml_diff>
--- a/src/downloads/PVS data - 060120.xlsx
+++ b/src/downloads/PVS data - 060120.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikevanmaele/Documents/GitHub/gida-landing/src/downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BDEAF70-D7B5-E74F-BD40-FA7F8C6C58CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC27E2B4-F72F-F149-9E9F-639C6BF79158}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5770,7 +5770,7 @@
         <v>81</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="38.5" customHeight="1" thickBot="1">

</xml_diff>

<commit_message>
Updated AMP download and security dataset downloads
</commit_message>
<xml_diff>
--- a/src/downloads/PVS data - 060120.xlsx
+++ b/src/downloads/PVS data - 060120.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikevanmaele/Documents/GitHub/gida-landing/src/downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natebennett/Documents/Talus/Code/IDEA/Landing/gida-landing/src/downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE69FB5-A313-C649-B5BA-3ED17EE5C812}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B49841-6E10-BB4E-BE46-AB917F8C876C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover page" sheetId="4" r:id="rId1"/>
@@ -1355,7 +1355,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1903,15 +1903,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2527301</xdr:colOff>
+      <xdr:colOff>698501</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:rowOff>646750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>5020510</xdr:colOff>
+      <xdr:colOff>6504023</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>2692400</xdr:rowOff>
+      <xdr:rowOff>2336800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1929,16 +1929,6 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:clrChange>
-            <a:clrFrom>
-              <a:srgbClr val="FFFFFF"/>
-            </a:clrFrom>
-            <a:clrTo>
-              <a:srgbClr val="FFFFFF">
-                <a:alpha val="0"/>
-              </a:srgbClr>
-            </a:clrTo>
-          </a:clrChange>
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1946,14 +1936,12 @@
           </a:extLst>
         </a:blip>
         <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2933701" y="330200"/>
-          <a:ext cx="2493209" cy="2552700"/>
+          <a:off x="1104901" y="837250"/>
+          <a:ext cx="5805522" cy="1690050"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1980,15 +1968,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>164671</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1054100</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>18143</xdr:rowOff>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1052531</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2005,15 +1993,20 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="4064000" cy="1161143"/>
+          <a:off x="164671" y="165100"/>
+          <a:ext cx="3048429" cy="887431"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2030,23 +2023,23 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>165100</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>4064000</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>18143</xdr:rowOff>
+      <xdr:colOff>3213529</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1052531</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB37DFC3-0760-5547-A1EA-DE09669AF9EE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46B71F71-082B-AC45-A618-FE76178E3A9B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2055,15 +2048,20 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="4064000" cy="1161143"/>
+          <a:off x="165100" y="165100"/>
+          <a:ext cx="3048429" cy="887431"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2080,23 +2078,23 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>165100</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>4064000</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>18143</xdr:rowOff>
+      <xdr:colOff>3213529</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1052531</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="5" name="Picture 4">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BD807AC-1FC7-8845-8BBA-15ED22BCF173}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B03FDE16-7AA4-0849-8BCC-B4A300CFE92C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2105,15 +2103,20 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="4064000" cy="1161143"/>
+          <a:off x="165100" y="165100"/>
+          <a:ext cx="3048429" cy="887431"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2130,23 +2133,23 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>165100</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>4064000</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>18143</xdr:rowOff>
+      <xdr:colOff>3213529</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1052531</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="5" name="Picture 4">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0741AF87-BF3B-1B4C-B9C8-A6A82FCBAFB7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40D09EB9-539B-CF40-AF1C-1C281B0A5B0A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2155,15 +2158,20 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="4064000" cy="1161143"/>
+          <a:off x="165100" y="165100"/>
+          <a:ext cx="3048429" cy="887431"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2180,23 +2188,23 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>165100</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>4064000</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>18143</xdr:rowOff>
+      <xdr:colOff>3213529</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1052531</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C422CAF-ED03-484E-AE7F-9BCE21DAC5F5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E5205E1-5ADF-8840-BDBB-75A90648DBCD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2205,15 +2213,20 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="4064000" cy="1161143"/>
+          <a:off x="165100" y="165100"/>
+          <a:ext cx="3048429" cy="887431"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2230,23 +2243,23 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>165100</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>4064000</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>18143</xdr:rowOff>
+      <xdr:colOff>3213529</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1052531</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFAA95B3-BD01-FA40-B540-2AF8266FF9C0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89C3D982-9E5F-5B48-A7A0-35A1F16F6F25}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2255,15 +2268,20 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="4064000" cy="1161143"/>
+          <a:off x="165100" y="165100"/>
+          <a:ext cx="3048429" cy="887431"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2280,23 +2298,23 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>165100</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>4064000</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>18143</xdr:rowOff>
+      <xdr:colOff>3213529</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1052531</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64BB8670-B136-4348-8F0F-82C81916B054}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5212186B-F2FD-FC40-9ED7-58D5A5B6AAA2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2305,15 +2323,20 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="4064000" cy="1161143"/>
+          <a:off x="165100" y="165100"/>
+          <a:ext cx="3048429" cy="887431"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2525,9 +2548,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{272FF391-350C-7040-AA4E-ABC7B5554BAA}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="2.6640625" customWidth="1"/>
     <col min="2" max="2" width="2.6640625" style="1" customWidth="1"/>
@@ -2537,27 +2562,27 @@
     <col min="19" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1"/>
-    <row r="2" spans="1:4" ht="216" customHeight="1">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:4" ht="216" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="7"/>
       <c r="C2" s="8"/>
       <c r="D2" s="9"/>
     </row>
-    <row r="3" spans="1:4" ht="79" customHeight="1">
+    <row r="3" spans="1:4" ht="79" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="10"/>
       <c r="C3" s="11" t="s">
         <v>368</v>
       </c>
       <c r="D3" s="12"/>
     </row>
-    <row r="4" spans="1:4" ht="33" customHeight="1">
+    <row r="4" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="10"/>
       <c r="C4" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="12"/>
     </row>
-    <row r="5" spans="1:4" s="6" customFormat="1" ht="209" customHeight="1" thickBot="1">
+    <row r="5" spans="1:4" s="6" customFormat="1" ht="209" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A5"/>
       <c r="B5" s="13"/>
       <c r="C5" s="19" t="s">
@@ -2565,7 +2590,7 @@
       </c>
       <c r="D5" s="14"/>
     </row>
-    <row r="6" spans="1:4" s="6" customFormat="1" ht="311" customHeight="1" thickBot="1">
+    <row r="6" spans="1:4" s="6" customFormat="1" ht="311" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6"/>
       <c r="B6" s="15"/>
       <c r="C6" s="18" t="s">
@@ -2585,10 +2610,10 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="39.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="52.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -2599,26 +2624,26 @@
     <col min="7" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="90" customHeight="1"/>
-    <row r="2" spans="1:6" ht="34">
+    <row r="1" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="2" spans="1:6" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="24">
+    <row r="3" spans="1:6" ht="24" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="70" customHeight="1">
+    <row r="4" spans="1:6" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="57" t="s">
         <v>116</v>
       </c>
       <c r="B4" s="57"/>
       <c r="C4" s="21"/>
     </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1"/>
-    <row r="6" spans="1:6" ht="77" customHeight="1" thickBot="1">
+    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:6" ht="77" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>29</v>
       </c>
@@ -2638,7 +2663,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="67" customHeight="1" thickBot="1">
+    <row r="7" spans="1:6" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>32</v>
       </c>
@@ -2656,7 +2681,7 @@
       </c>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="67" customHeight="1" thickBot="1">
+    <row r="8" spans="1:6" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>36</v>
       </c>
@@ -2674,7 +2699,7 @@
       </c>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" ht="67" customHeight="1" thickBot="1">
+    <row r="9" spans="1:6" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>38</v>
       </c>
@@ -2692,7 +2717,7 @@
       </c>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" ht="67" customHeight="1" thickBot="1">
+    <row r="10" spans="1:6" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>39</v>
       </c>
@@ -2710,7 +2735,7 @@
       </c>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" ht="67" customHeight="1" thickBot="1">
+    <row r="11" spans="1:6" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>42</v>
       </c>
@@ -2728,7 +2753,7 @@
       </c>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" ht="67" customHeight="1" thickBot="1">
+    <row r="12" spans="1:6" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>44</v>
       </c>
@@ -2746,7 +2771,7 @@
       </c>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" ht="67" customHeight="1" thickBot="1">
+    <row r="13" spans="1:6" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>47</v>
       </c>
@@ -2764,7 +2789,7 @@
       </c>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" ht="67" customHeight="1" thickBot="1">
+    <row r="14" spans="1:6" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>47</v>
       </c>
@@ -2782,7 +2807,7 @@
       </c>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6" ht="67" customHeight="1" thickBot="1">
+    <row r="15" spans="1:6" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>54</v>
       </c>
@@ -2800,7 +2825,7 @@
       </c>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:6" ht="67" customHeight="1" thickBot="1">
+    <row r="16" spans="1:6" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>57</v>
       </c>
@@ -2818,7 +2843,7 @@
       </c>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6" ht="67" customHeight="1" thickBot="1">
+    <row r="17" spans="1:6" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>59</v>
       </c>
@@ -2836,7 +2861,7 @@
       </c>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6" ht="67" customHeight="1" thickBot="1">
+    <row r="18" spans="1:6" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>61</v>
       </c>
@@ -2854,7 +2879,7 @@
       </c>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" ht="67" customHeight="1" thickBot="1">
+    <row r="19" spans="1:6" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>65</v>
       </c>
@@ -2872,7 +2897,7 @@
       </c>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:6" ht="67" customHeight="1" thickBot="1">
+    <row r="20" spans="1:6" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>68</v>
       </c>
@@ -2890,7 +2915,7 @@
       </c>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" ht="67" customHeight="1" thickBot="1">
+    <row r="21" spans="1:6" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>70</v>
       </c>
@@ -2910,7 +2935,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="67" customHeight="1" thickBot="1">
+    <row r="22" spans="1:6" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>73</v>
       </c>
@@ -2928,7 +2953,7 @@
       </c>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:6" ht="67" customHeight="1" thickBot="1">
+    <row r="23" spans="1:6" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>75</v>
       </c>
@@ -2946,7 +2971,7 @@
       </c>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:6" ht="67" customHeight="1" thickBot="1">
+    <row r="24" spans="1:6" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>77</v>
       </c>
@@ -2964,7 +2989,7 @@
       </c>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:6" ht="67" customHeight="1" thickBot="1">
+    <row r="25" spans="1:6" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>79</v>
       </c>
@@ -2982,7 +3007,7 @@
       </c>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6" ht="67" customHeight="1" thickBot="1">
+    <row r="26" spans="1:6" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>81</v>
       </c>
@@ -3000,7 +3025,7 @@
       </c>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="1:6" ht="67" customHeight="1" thickBot="1">
+    <row r="27" spans="1:6" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>83</v>
       </c>
@@ -3018,7 +3043,7 @@
       </c>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="1:6" ht="67" customHeight="1" thickBot="1">
+    <row r="28" spans="1:6" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>85</v>
       </c>
@@ -3036,7 +3061,7 @@
       </c>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:6" ht="67" customHeight="1" thickBot="1">
+    <row r="29" spans="1:6" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>86</v>
       </c>
@@ -3054,7 +3079,7 @@
       </c>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:6" ht="67" customHeight="1" thickBot="1">
+    <row r="30" spans="1:6" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>88</v>
       </c>
@@ -3072,7 +3097,7 @@
       </c>
       <c r="F30" s="5"/>
     </row>
-    <row r="31" spans="1:6" ht="67" customHeight="1" thickBot="1">
+    <row r="31" spans="1:6" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>91</v>
       </c>
@@ -3090,7 +3115,7 @@
       </c>
       <c r="F31" s="5"/>
     </row>
-    <row r="32" spans="1:6" ht="67" customHeight="1" thickBot="1">
+    <row r="32" spans="1:6" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>93</v>
       </c>
@@ -3108,7 +3133,7 @@
       </c>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:6" ht="67" customHeight="1" thickBot="1">
+    <row r="33" spans="1:6" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>95</v>
       </c>
@@ -3126,7 +3151,7 @@
       </c>
       <c r="F33" s="5"/>
     </row>
-    <row r="34" spans="1:6" ht="67" customHeight="1" thickBot="1">
+    <row r="34" spans="1:6" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>97</v>
       </c>
@@ -3144,7 +3169,7 @@
       </c>
       <c r="F34" s="5"/>
     </row>
-    <row r="35" spans="1:6" ht="67" customHeight="1" thickBot="1">
+    <row r="35" spans="1:6" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>99</v>
       </c>
@@ -3162,7 +3187,7 @@
       </c>
       <c r="F35" s="5"/>
     </row>
-    <row r="36" spans="1:6" ht="67" customHeight="1" thickBot="1">
+    <row r="36" spans="1:6" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>101</v>
       </c>
@@ -3180,7 +3205,7 @@
       </c>
       <c r="F36" s="5"/>
     </row>
-    <row r="37" spans="1:6" ht="67" customHeight="1" thickBot="1">
+    <row r="37" spans="1:6" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>103</v>
       </c>
@@ -3198,7 +3223,7 @@
       </c>
       <c r="F37" s="5"/>
     </row>
-    <row r="38" spans="1:6" ht="67" customHeight="1" thickBot="1">
+    <row r="38" spans="1:6" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
         <v>106</v>
       </c>
@@ -3216,7 +3241,7 @@
       </c>
       <c r="F38" s="5"/>
     </row>
-    <row r="39" spans="1:6" ht="67" customHeight="1" thickBot="1">
+    <row r="39" spans="1:6" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
         <v>109</v>
       </c>
@@ -3234,7 +3259,7 @@
       </c>
       <c r="F39" s="5"/>
     </row>
-    <row r="40" spans="1:6" ht="67" customHeight="1" thickBot="1">
+    <row r="40" spans="1:6" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>111</v>
       </c>
@@ -3310,36 +3335,36 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="73" style="1" customWidth="1"/>
     <col min="2" max="3" width="42.1640625" style="1" customWidth="1"/>
     <col min="4" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="90" customHeight="1"/>
-    <row r="2" spans="1:3" ht="34">
+    <row r="1" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="24">
+    <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="70" customHeight="1">
+    <row r="4" spans="1:3" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="57" t="s">
         <v>363</v>
       </c>
       <c r="B4" s="57"/>
       <c r="C4" s="21"/>
     </row>
-    <row r="5" spans="1:3" ht="15" thickBot="1"/>
-    <row r="6" spans="1:3" ht="38.5" customHeight="1" thickBot="1">
+    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:3" ht="38.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>120</v>
       </c>
@@ -3347,7 +3372,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="38.5" customHeight="1" thickBot="1">
+    <row r="7" spans="1:3" ht="38.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
         <v>119</v>
       </c>
@@ -3358,21 +3383,21 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="8" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A8" s="26" t="s">
         <v>121</v>
       </c>
       <c r="B8" s="23"/>
       <c r="C8" s="24"/>
     </row>
-    <row r="9" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="9" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A9" s="37" t="s">
         <v>345</v>
       </c>
       <c r="B9" s="45"/>
       <c r="C9" s="46"/>
     </row>
-    <row r="10" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="10" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="40" t="s">
         <v>122</v>
       </c>
@@ -3383,7 +3408,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="11" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="38" t="s">
         <v>123</v>
       </c>
@@ -3394,14 +3419,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="12" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A12" s="37" t="s">
         <v>346</v>
       </c>
       <c r="B12" s="45"/>
       <c r="C12" s="46"/>
     </row>
-    <row r="13" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="13" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" s="38" t="s">
         <v>124</v>
       </c>
@@ -3412,7 +3437,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="14" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A14" s="38" t="s">
         <v>125</v>
       </c>
@@ -3423,7 +3448,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="15" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>352</v>
       </c>
@@ -3434,7 +3459,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="16" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
         <v>126</v>
       </c>
@@ -3445,7 +3470,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="17" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A17" s="36" t="s">
         <v>127</v>
       </c>
@@ -3456,14 +3481,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="18" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A18" s="37" t="s">
         <v>347</v>
       </c>
       <c r="B18" s="45"/>
       <c r="C18" s="46"/>
     </row>
-    <row r="19" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="19" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A19" s="38" t="s">
         <v>168</v>
       </c>
@@ -3474,7 +3499,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="20" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A20" s="38" t="s">
         <v>353</v>
       </c>
@@ -3485,7 +3510,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="21" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A21" s="36" t="s">
         <v>354</v>
       </c>
@@ -3496,7 +3521,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="22" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A22" s="36" t="s">
         <v>128</v>
       </c>
@@ -3507,7 +3532,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="23" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A23" s="39" t="s">
         <v>129</v>
       </c>
@@ -3518,21 +3543,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="24" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A24" s="26" t="s">
         <v>130</v>
       </c>
       <c r="B24" s="31"/>
       <c r="C24" s="32"/>
     </row>
-    <row r="25" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="25" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A25" s="37" t="s">
         <v>337</v>
       </c>
       <c r="B25" s="45"/>
       <c r="C25" s="46"/>
     </row>
-    <row r="26" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="26" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A26" s="40" t="s">
         <v>131</v>
       </c>
@@ -3543,7 +3568,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="27" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A27" s="38" t="s">
         <v>132</v>
       </c>
@@ -3554,7 +3579,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="28" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A28" s="38" t="s">
         <v>133</v>
       </c>
@@ -3565,7 +3590,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="29" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A29" s="36" t="s">
         <v>355</v>
       </c>
@@ -3576,7 +3601,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="30" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A30" s="36" t="s">
         <v>356</v>
       </c>
@@ -3587,14 +3612,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="31" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A31" s="37" t="s">
         <v>348</v>
       </c>
       <c r="B31" s="45"/>
       <c r="C31" s="46"/>
     </row>
-    <row r="32" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="32" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A32" s="38" t="s">
         <v>134</v>
       </c>
@@ -3605,7 +3630,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="33" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A33" s="38" t="s">
         <v>135</v>
       </c>
@@ -3616,7 +3641,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="34" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A34" s="36" t="s">
         <v>136</v>
       </c>
@@ -3627,7 +3652,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="35" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A35" s="36" t="s">
         <v>137</v>
       </c>
@@ -3638,14 +3663,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="36" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A36" s="37" t="s">
         <v>349</v>
       </c>
       <c r="B36" s="45"/>
       <c r="C36" s="46"/>
     </row>
-    <row r="37" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="37" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A37" s="38" t="s">
         <v>138</v>
       </c>
@@ -3656,7 +3681,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="38" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A38" s="38" t="s">
         <v>139</v>
       </c>
@@ -3667,7 +3692,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="39" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A39" s="36" t="s">
         <v>357</v>
       </c>
@@ -3678,7 +3703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="40" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A40" s="36" t="s">
         <v>140</v>
       </c>
@@ -3689,7 +3714,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="41" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A41" s="36" t="s">
         <v>141</v>
       </c>
@@ -3700,7 +3725,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="42" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A42" s="36" t="s">
         <v>142</v>
       </c>
@@ -3711,14 +3736,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="43" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A43" s="37" t="s">
         <v>350</v>
       </c>
       <c r="B43" s="45"/>
       <c r="C43" s="46"/>
     </row>
-    <row r="44" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="44" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A44" s="38" t="s">
         <v>143</v>
       </c>
@@ -3729,7 +3754,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="45" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A45" s="38" t="s">
         <v>144</v>
       </c>
@@ -3740,7 +3765,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="46" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A46" s="39" t="s">
         <v>145</v>
       </c>
@@ -3751,14 +3776,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="47" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A47" s="26" t="s">
         <v>146</v>
       </c>
       <c r="B47" s="31"/>
       <c r="C47" s="32"/>
     </row>
-    <row r="48" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="48" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A48" s="49" t="s">
         <v>147</v>
       </c>
@@ -3769,7 +3794,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="49" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A49" s="36" t="s">
         <v>148</v>
       </c>
@@ -3780,7 +3805,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="50" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A50" s="36" t="s">
         <v>149</v>
       </c>
@@ -3791,7 +3816,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="51" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A51" s="36" t="s">
         <v>150</v>
       </c>
@@ -3802,7 +3827,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="52" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A52" s="36" t="s">
         <v>151</v>
       </c>
@@ -3813,7 +3838,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="53" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A53" s="36" t="s">
         <v>152</v>
       </c>
@@ -3824,7 +3849,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="54" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A54" s="39" t="s">
         <v>153</v>
       </c>
@@ -3835,21 +3860,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="55" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A55" s="26" t="s">
         <v>154</v>
       </c>
       <c r="B55" s="31"/>
       <c r="C55" s="32"/>
     </row>
-    <row r="56" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="56" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A56" s="37" t="s">
         <v>351</v>
       </c>
       <c r="B56" s="45"/>
       <c r="C56" s="46"/>
     </row>
-    <row r="57" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="57" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A57" s="40" t="s">
         <v>155</v>
       </c>
@@ -3860,7 +3885,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="58" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A58" s="38" t="s">
         <v>156</v>
       </c>
@@ -3871,7 +3896,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="59" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A59" s="36" t="s">
         <v>157</v>
       </c>
@@ -3882,7 +3907,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="60" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A60" s="36" t="s">
         <v>158</v>
       </c>
@@ -3893,7 +3918,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="61" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A61" s="36" t="s">
         <v>159</v>
       </c>
@@ -3904,7 +3929,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="62" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A62" s="36" t="s">
         <v>160</v>
       </c>
@@ -3915,7 +3940,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="63" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A63" s="36" t="s">
         <v>161</v>
       </c>
@@ -3926,7 +3951,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="64" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A64" s="36" t="s">
         <v>162</v>
       </c>
@@ -3953,36 +3978,36 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="73" style="1" customWidth="1"/>
     <col min="2" max="10" width="42.1640625" style="1" customWidth="1"/>
     <col min="11" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="90" customHeight="1"/>
-    <row r="2" spans="1:10" ht="34">
+    <row r="1" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="2" spans="1:10" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="24">
+    <row r="3" spans="1:10" ht="24" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="70" customHeight="1">
+    <row r="4" spans="1:10" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="57" t="s">
         <v>362</v>
       </c>
       <c r="B4" s="57"/>
       <c r="C4" s="21"/>
     </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1"/>
-    <row r="6" spans="1:10" ht="38.5" customHeight="1" thickBot="1">
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:10" ht="38.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>32</v>
       </c>
@@ -4011,7 +4036,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="38.5" customHeight="1" thickBot="1">
+    <row r="7" spans="1:10" ht="38.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
         <v>119</v>
       </c>
@@ -4043,7 +4068,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="8" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A8" s="26" t="s">
         <v>121</v>
       </c>
@@ -4057,7 +4082,7 @@
       <c r="I8" s="23"/>
       <c r="J8" s="24"/>
     </row>
-    <row r="9" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="9" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A9" s="37" t="s">
         <v>334</v>
       </c>
@@ -4071,7 +4096,7 @@
       <c r="I9" s="45"/>
       <c r="J9" s="46"/>
     </row>
-    <row r="10" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="10" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="40" t="s">
         <v>207</v>
       </c>
@@ -4103,7 +4128,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="11" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="38" t="s">
         <v>208</v>
       </c>
@@ -4135,7 +4160,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="12" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A12" s="37" t="s">
         <v>335</v>
       </c>
@@ -4149,7 +4174,7 @@
       <c r="I12" s="45"/>
       <c r="J12" s="46"/>
     </row>
-    <row r="13" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="13" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" s="38" t="s">
         <v>209</v>
       </c>
@@ -4181,7 +4206,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="14" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A14" s="38" t="s">
         <v>210</v>
       </c>
@@ -4213,7 +4238,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="15" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>166</v>
       </c>
@@ -4245,7 +4270,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="16" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
         <v>126</v>
       </c>
@@ -4277,7 +4302,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="17" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A17" s="36" t="s">
         <v>167</v>
       </c>
@@ -4309,7 +4334,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="18" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A18" s="37" t="s">
         <v>336</v>
       </c>
@@ -4323,7 +4348,7 @@
       <c r="I18" s="45"/>
       <c r="J18" s="46"/>
     </row>
-    <row r="19" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="19" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A19" s="38" t="s">
         <v>168</v>
       </c>
@@ -4355,7 +4380,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="20" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A20" s="38" t="s">
         <v>169</v>
       </c>
@@ -4387,7 +4412,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="21" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A21" s="36" t="s">
         <v>170</v>
       </c>
@@ -4419,7 +4444,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="22" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A22" s="36" t="s">
         <v>171</v>
       </c>
@@ -4451,7 +4476,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="23" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A23" s="39" t="s">
         <v>172</v>
       </c>
@@ -4483,7 +4508,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="24" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A24" s="39" t="s">
         <v>173</v>
       </c>
@@ -4515,7 +4540,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="25" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A25" s="39" t="s">
         <v>174</v>
       </c>
@@ -4547,7 +4572,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="25" customFormat="1" ht="67" customHeight="1" thickBot="1">
+    <row r="26" spans="1:10" s="25" customFormat="1" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A26" s="26" t="s">
         <v>175</v>
       </c>
@@ -4561,7 +4586,7 @@
       <c r="I26" s="27"/>
       <c r="J26" s="28"/>
     </row>
-    <row r="27" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="27" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A27" s="37" t="s">
         <v>337</v>
       </c>
@@ -4575,7 +4600,7 @@
       <c r="I27" s="45"/>
       <c r="J27" s="46"/>
     </row>
-    <row r="28" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="28" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A28" s="40" t="s">
         <v>211</v>
       </c>
@@ -4607,7 +4632,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="29" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A29" s="38" t="s">
         <v>212</v>
       </c>
@@ -4639,7 +4664,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="30" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A30" s="36" t="s">
         <v>177</v>
       </c>
@@ -4671,7 +4696,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="31" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A31" s="36" t="s">
         <v>178</v>
       </c>
@@ -4703,7 +4728,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="32" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A32" s="36" t="s">
         <v>179</v>
       </c>
@@ -4735,7 +4760,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="33" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A33" s="37" t="s">
         <v>338</v>
       </c>
@@ -4749,7 +4774,7 @@
       <c r="I33" s="45"/>
       <c r="J33" s="46"/>
     </row>
-    <row r="34" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="34" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A34" s="38" t="s">
         <v>213</v>
       </c>
@@ -4781,7 +4806,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="35" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A35" s="38" t="s">
         <v>214</v>
       </c>
@@ -4813,7 +4838,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="36" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A36" s="36" t="s">
         <v>215</v>
       </c>
@@ -4845,7 +4870,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="37" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A37" s="36" t="s">
         <v>181</v>
       </c>
@@ -4877,7 +4902,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="38" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A38" s="37" t="s">
         <v>339</v>
       </c>
@@ -4891,7 +4916,7 @@
       <c r="I38" s="45"/>
       <c r="J38" s="46"/>
     </row>
-    <row r="39" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="39" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A39" s="38" t="s">
         <v>216</v>
       </c>
@@ -4923,7 +4948,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="40" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A40" s="38" t="s">
         <v>217</v>
       </c>
@@ -4955,7 +4980,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="41" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A41" s="38" t="s">
         <v>218</v>
       </c>
@@ -4987,7 +5012,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="42" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A42" s="36" t="s">
         <v>184</v>
       </c>
@@ -5019,7 +5044,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="43" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A43" s="36" t="s">
         <v>185</v>
       </c>
@@ -5051,7 +5076,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="44" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A44" s="36" t="s">
         <v>219</v>
       </c>
@@ -5083,7 +5108,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="45" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A45" s="37" t="s">
         <v>340</v>
       </c>
@@ -5097,7 +5122,7 @@
       <c r="I45" s="45"/>
       <c r="J45" s="46"/>
     </row>
-    <row r="46" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="46" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A46" s="51" t="s">
         <v>220</v>
       </c>
@@ -5129,7 +5154,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="47" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A47" s="51" t="s">
         <v>221</v>
       </c>
@@ -5161,7 +5186,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="48" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A48" s="39" t="s">
         <v>145</v>
       </c>
@@ -5193,7 +5218,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="49" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A49" s="26" t="s">
         <v>222</v>
       </c>
@@ -5207,7 +5232,7 @@
       <c r="I49" s="27"/>
       <c r="J49" s="28"/>
     </row>
-    <row r="50" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="50" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A50" s="49" t="s">
         <v>192</v>
       </c>
@@ -5239,7 +5264,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="51" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A51" s="36" t="s">
         <v>223</v>
       </c>
@@ -5271,7 +5296,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="52" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A52" s="36" t="s">
         <v>194</v>
       </c>
@@ -5303,7 +5328,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="53" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A53" s="36" t="s">
         <v>364</v>
       </c>
@@ -5335,7 +5360,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="54" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A54" s="37" t="s">
         <v>341</v>
       </c>
@@ -5349,7 +5374,7 @@
       <c r="I54" s="45"/>
       <c r="J54" s="46"/>
     </row>
-    <row r="55" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="55" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A55" s="51" t="s">
         <v>195</v>
       </c>
@@ -5381,7 +5406,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="56" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A56" s="51" t="s">
         <v>196</v>
       </c>
@@ -5413,7 +5438,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="57" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A57" s="39" t="s">
         <v>224</v>
       </c>
@@ -5445,7 +5470,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="58" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A58" s="26" t="s">
         <v>198</v>
       </c>
@@ -5459,7 +5484,7 @@
       <c r="I58" s="27"/>
       <c r="J58" s="28"/>
     </row>
-    <row r="59" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="59" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A59" s="49" t="s">
         <v>199</v>
       </c>
@@ -5491,7 +5516,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="60" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A60" s="36" t="s">
         <v>225</v>
       </c>
@@ -5523,7 +5548,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="61" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A61" s="36" t="s">
         <v>201</v>
       </c>
@@ -5555,7 +5580,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="62" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A62" s="36" t="s">
         <v>202</v>
       </c>
@@ -5587,7 +5612,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="63" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A63" s="36" t="s">
         <v>203</v>
       </c>
@@ -5619,7 +5644,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="64" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A64" s="36" t="s">
         <v>204</v>
       </c>
@@ -5651,7 +5676,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="65" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A65" s="36" t="s">
         <v>226</v>
       </c>
@@ -5683,7 +5708,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="67" customHeight="1" thickBot="1">
+    <row r="66" spans="1:10" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A66" s="36" t="s">
         <v>227</v>
       </c>
@@ -5731,36 +5756,36 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="73" style="1" customWidth="1"/>
     <col min="2" max="7" width="42.1640625" style="1" customWidth="1"/>
     <col min="8" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="90" customHeight="1"/>
-    <row r="2" spans="1:7" ht="34">
+    <row r="1" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="2" spans="1:7" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="24">
+    <row r="3" spans="1:7" ht="24" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="70" customHeight="1">
+    <row r="4" spans="1:7" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="57" t="s">
         <v>361</v>
       </c>
       <c r="B4" s="57"/>
       <c r="C4" s="21"/>
     </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1"/>
-    <row r="6" spans="1:7" ht="38.5" customHeight="1" thickBot="1">
+    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:7" ht="38.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>99</v>
       </c>
@@ -5780,7 +5805,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="38.5" customHeight="1" thickBot="1">
+    <row r="7" spans="1:7" ht="38.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
         <v>119</v>
       </c>
@@ -5803,7 +5828,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="8" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A8" s="26" t="s">
         <v>121</v>
       </c>
@@ -5814,7 +5839,7 @@
       <c r="F8" s="29"/>
       <c r="G8" s="30"/>
     </row>
-    <row r="9" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="9" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A9" s="37" t="s">
         <v>334</v>
       </c>
@@ -5825,7 +5850,7 @@
       <c r="F9" s="52"/>
       <c r="G9" s="53"/>
     </row>
-    <row r="10" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="10" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="40" t="s">
         <v>207</v>
       </c>
@@ -5848,7 +5873,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="11" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="51" t="s">
         <v>208</v>
       </c>
@@ -5871,7 +5896,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="12" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A12" s="37" t="s">
         <v>335</v>
       </c>
@@ -5882,7 +5907,7 @@
       <c r="F12" s="52"/>
       <c r="G12" s="53"/>
     </row>
-    <row r="13" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="13" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" s="40" t="s">
         <v>209</v>
       </c>
@@ -5905,7 +5930,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="14" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A14" s="38" t="s">
         <v>210</v>
       </c>
@@ -5928,7 +5953,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="15" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>166</v>
       </c>
@@ -5951,7 +5976,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="16" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
         <v>126</v>
       </c>
@@ -5974,7 +5999,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="17" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A17" s="36" t="s">
         <v>167</v>
       </c>
@@ -5997,7 +6022,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="18" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A18" s="37" t="s">
         <v>336</v>
       </c>
@@ -6008,7 +6033,7 @@
       <c r="F18" s="52"/>
       <c r="G18" s="53"/>
     </row>
-    <row r="19" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="19" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A19" s="38" t="s">
         <v>168</v>
       </c>
@@ -6031,7 +6056,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="20" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A20" s="38" t="s">
         <v>169</v>
       </c>
@@ -6054,7 +6079,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="21" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A21" s="39" t="s">
         <v>170</v>
       </c>
@@ -6077,7 +6102,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="22" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A22" s="36" t="s">
         <v>171</v>
       </c>
@@ -6100,7 +6125,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="23" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A23" s="49" t="s">
         <v>172</v>
       </c>
@@ -6123,7 +6148,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="24" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A24" s="36" t="s">
         <v>173</v>
       </c>
@@ -6146,7 +6171,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="25" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A25" s="39" t="s">
         <v>174</v>
       </c>
@@ -6169,7 +6194,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="26" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A26" s="26" t="s">
         <v>175</v>
       </c>
@@ -6180,7 +6205,7 @@
       <c r="F26" s="27"/>
       <c r="G26" s="28"/>
     </row>
-    <row r="27" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="27" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A27" s="49" t="s">
         <v>176</v>
       </c>
@@ -6203,7 +6228,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="28" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A28" s="36" t="s">
         <v>177</v>
       </c>
@@ -6226,7 +6251,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="29" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A29" s="36" t="s">
         <v>178</v>
       </c>
@@ -6249,7 +6274,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="30" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A30" s="39" t="s">
         <v>179</v>
       </c>
@@ -6272,7 +6297,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="31" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A31" s="37" t="s">
         <v>342</v>
       </c>
@@ -6283,7 +6308,7 @@
       <c r="F31" s="52"/>
       <c r="G31" s="53"/>
     </row>
-    <row r="32" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="32" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A32" s="40" t="s">
         <v>213</v>
       </c>
@@ -6306,7 +6331,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="33" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A33" s="38" t="s">
         <v>214</v>
       </c>
@@ -6329,7 +6354,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="34" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A34" s="36" t="s">
         <v>180</v>
       </c>
@@ -6352,7 +6377,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="35" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A35" s="36" t="s">
         <v>181</v>
       </c>
@@ -6375,7 +6400,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="36" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A36" s="37" t="s">
         <v>343</v>
       </c>
@@ -6386,7 +6411,7 @@
       <c r="F36" s="52"/>
       <c r="G36" s="53"/>
     </row>
-    <row r="37" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="37" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A37" s="38" t="s">
         <v>182</v>
       </c>
@@ -6409,7 +6434,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="38" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A38" s="38" t="s">
         <v>183</v>
       </c>
@@ -6432,7 +6457,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="39" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A39" s="36" t="s">
         <v>184</v>
       </c>
@@ -6455,7 +6480,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="40" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A40" s="36" t="s">
         <v>185</v>
       </c>
@@ -6478,7 +6503,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="41" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A41" s="39" t="s">
         <v>186</v>
       </c>
@@ -6501,7 +6526,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="42" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A42" s="39" t="s">
         <v>187</v>
       </c>
@@ -6524,7 +6549,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="43" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A43" s="37" t="s">
         <v>344</v>
       </c>
@@ -6535,7 +6560,7 @@
       <c r="F43" s="52"/>
       <c r="G43" s="53"/>
     </row>
-    <row r="44" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="44" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A44" s="51" t="s">
         <v>188</v>
       </c>
@@ -6558,7 +6583,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="45" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A45" s="51" t="s">
         <v>189</v>
       </c>
@@ -6581,7 +6606,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="46" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A46" s="39" t="s">
         <v>190</v>
       </c>
@@ -6604,7 +6629,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="47" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A47" s="26" t="s">
         <v>191</v>
       </c>
@@ -6615,7 +6640,7 @@
       <c r="F47" s="27"/>
       <c r="G47" s="28"/>
     </row>
-    <row r="48" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="48" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A48" s="49" t="s">
         <v>192</v>
       </c>
@@ -6638,7 +6663,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="49" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A49" s="36" t="s">
         <v>193</v>
       </c>
@@ -6661,7 +6686,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="50" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A50" s="36" t="s">
         <v>194</v>
       </c>
@@ -6684,7 +6709,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="51" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A51" s="36" t="s">
         <v>365</v>
       </c>
@@ -6707,7 +6732,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="52" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A52" s="37" t="s">
         <v>341</v>
       </c>
@@ -6718,7 +6743,7 @@
       <c r="F52" s="52"/>
       <c r="G52" s="53"/>
     </row>
-    <row r="53" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="53" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A53" s="38" t="s">
         <v>195</v>
       </c>
@@ -6741,7 +6766,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="54" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A54" s="38" t="s">
         <v>196</v>
       </c>
@@ -6764,7 +6789,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="55" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A55" s="39" t="s">
         <v>197</v>
       </c>
@@ -6787,7 +6812,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="56" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A56" s="26" t="s">
         <v>198</v>
       </c>
@@ -6798,7 +6823,7 @@
       <c r="F56" s="27"/>
       <c r="G56" s="28"/>
     </row>
-    <row r="57" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="57" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A57" s="49" t="s">
         <v>199</v>
       </c>
@@ -6821,7 +6846,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="58" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A58" s="36" t="s">
         <v>200</v>
       </c>
@@ -6844,7 +6869,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="59" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A59" s="36" t="s">
         <v>201</v>
       </c>
@@ -6867,7 +6892,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="60" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A60" s="36" t="s">
         <v>202</v>
       </c>
@@ -6890,7 +6915,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="61" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A61" s="36" t="s">
         <v>203</v>
       </c>
@@ -6913,7 +6938,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="62" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A62" s="36" t="s">
         <v>204</v>
       </c>
@@ -6936,7 +6961,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="63" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A63" s="36" t="s">
         <v>205</v>
       </c>
@@ -6959,7 +6984,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="67" customHeight="1" thickBot="1">
+    <row r="64" spans="1:7" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A64" s="36" t="s">
         <v>206</v>
       </c>
@@ -6998,36 +7023,36 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="73" style="1" customWidth="1"/>
     <col min="2" max="8" width="42.1640625" style="1" customWidth="1"/>
     <col min="9" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="90" customHeight="1"/>
-    <row r="2" spans="1:8" ht="34">
+    <row r="1" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="2" spans="1:8" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="24">
+    <row r="3" spans="1:8" ht="24" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="70" customHeight="1">
+    <row r="4" spans="1:8" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="57" t="s">
         <v>360</v>
       </c>
       <c r="B4" s="57"/>
       <c r="C4" s="21"/>
     </row>
-    <row r="5" spans="1:8" ht="15" thickBot="1"/>
-    <row r="6" spans="1:8" ht="38.5" customHeight="1" thickBot="1">
+    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:8" ht="38.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>86</v>
       </c>
@@ -7050,7 +7075,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="38.5" customHeight="1" thickBot="1">
+    <row r="7" spans="1:8" ht="38.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
         <v>119</v>
       </c>
@@ -7076,7 +7101,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="8" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A8" s="26" t="s">
         <v>121</v>
       </c>
@@ -7088,7 +7113,7 @@
       <c r="G8" s="23"/>
       <c r="H8" s="24"/>
     </row>
-    <row r="9" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="9" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A9" s="37" t="s">
         <v>334</v>
       </c>
@@ -7100,7 +7125,7 @@
       <c r="G9" s="52"/>
       <c r="H9" s="53"/>
     </row>
-    <row r="10" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="10" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="40" t="s">
         <v>329</v>
       </c>
@@ -7126,7 +7151,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="11" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="51" t="s">
         <v>330</v>
       </c>
@@ -7152,7 +7177,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="12" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A12" s="37" t="s">
         <v>335</v>
       </c>
@@ -7164,7 +7189,7 @@
       <c r="G12" s="52"/>
       <c r="H12" s="53"/>
     </row>
-    <row r="13" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="13" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" s="40" t="s">
         <v>209</v>
       </c>
@@ -7190,7 +7215,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="14" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A14" s="38" t="s">
         <v>331</v>
       </c>
@@ -7216,7 +7241,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="15" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>232</v>
       </c>
@@ -7242,7 +7267,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="16" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
         <v>233</v>
       </c>
@@ -7268,7 +7293,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="17" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A17" s="36" t="s">
         <v>234</v>
       </c>
@@ -7294,7 +7319,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="18" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A18" s="36" t="s">
         <v>235</v>
       </c>
@@ -7320,7 +7345,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="19" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A19" s="36" t="s">
         <v>236</v>
       </c>
@@ -7346,7 +7371,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="20" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A20" s="36" t="s">
         <v>237</v>
       </c>
@@ -7372,7 +7397,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="21" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A21" s="36" t="s">
         <v>238</v>
       </c>
@@ -7398,7 +7423,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="22" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A22" s="36" t="s">
         <v>239</v>
       </c>
@@ -7424,7 +7449,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="23" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A23" s="26" t="s">
         <v>175</v>
       </c>
@@ -7436,7 +7461,7 @@
       <c r="G23" s="27"/>
       <c r="H23" s="28"/>
     </row>
-    <row r="24" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="24" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A24" s="49" t="s">
         <v>240</v>
       </c>
@@ -7462,7 +7487,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="25" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A25" s="36" t="s">
         <v>241</v>
       </c>
@@ -7488,7 +7513,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="26" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A26" s="36" t="s">
         <v>242</v>
       </c>
@@ -7514,7 +7539,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="27" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A27" s="36" t="s">
         <v>243</v>
       </c>
@@ -7540,7 +7565,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="28" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A28" s="37" t="s">
         <v>342</v>
       </c>
@@ -7552,7 +7577,7 @@
       <c r="G28" s="52"/>
       <c r="H28" s="53"/>
     </row>
-    <row r="29" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="29" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A29" s="38" t="s">
         <v>213</v>
       </c>
@@ -7578,7 +7603,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="30" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A30" s="38" t="s">
         <v>214</v>
       </c>
@@ -7604,7 +7629,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="31" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A31" s="36" t="s">
         <v>244</v>
       </c>
@@ -7630,7 +7655,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="32" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A32" s="36" t="s">
         <v>245</v>
       </c>
@@ -7656,7 +7681,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="33" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A33" s="36" t="s">
         <v>246</v>
       </c>
@@ -7682,7 +7707,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="34" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A34" s="36" t="s">
         <v>247</v>
       </c>
@@ -7708,7 +7733,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="35" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A35" s="36" t="s">
         <v>248</v>
       </c>
@@ -7734,7 +7759,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="36" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A36" s="36" t="s">
         <v>249</v>
       </c>
@@ -7760,7 +7785,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="37" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A37" s="39" t="s">
         <v>250</v>
       </c>
@@ -7786,7 +7811,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="38" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A38" s="26" t="s">
         <v>191</v>
       </c>
@@ -7798,7 +7823,7 @@
       <c r="G38" s="27"/>
       <c r="H38" s="28"/>
     </row>
-    <row r="39" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="39" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A39" s="49" t="s">
         <v>251</v>
       </c>
@@ -7824,7 +7849,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="40" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A40" s="39" t="s">
         <v>252</v>
       </c>
@@ -7850,7 +7875,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="41" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A41" s="39" t="s">
         <v>253</v>
       </c>
@@ -7876,7 +7901,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="42" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A42" s="39" t="s">
         <v>366</v>
       </c>
@@ -7902,7 +7927,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="43" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A43" s="39" t="s">
         <v>254</v>
       </c>
@@ -7928,7 +7953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="44" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A44" s="39" t="s">
         <v>255</v>
       </c>
@@ -7954,7 +7979,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="45" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A45" s="26" t="s">
         <v>198</v>
       </c>
@@ -7966,7 +7991,7 @@
       <c r="G45" s="27"/>
       <c r="H45" s="28"/>
     </row>
-    <row r="46" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="46" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A46" s="49" t="s">
         <v>256</v>
       </c>
@@ -7992,7 +8017,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="47" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A47" s="36" t="s">
         <v>257</v>
       </c>
@@ -8018,7 +8043,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="48" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A48" s="39" t="s">
         <v>258</v>
       </c>
@@ -8044,7 +8069,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="49" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A49" s="39" t="s">
         <v>259</v>
       </c>
@@ -8070,7 +8095,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="50" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A50" s="39" t="s">
         <v>260</v>
       </c>
@@ -8096,7 +8121,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="51" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A51" s="39" t="s">
         <v>261</v>
       </c>
@@ -8122,7 +8147,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="52" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A52" s="36" t="s">
         <v>262</v>
       </c>
@@ -8148,7 +8173,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="53" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A53" s="36" t="s">
         <v>263</v>
       </c>
@@ -8174,7 +8199,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="54" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A54" s="36" t="s">
         <v>264</v>
       </c>
@@ -8216,36 +8241,36 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="73" style="1" customWidth="1"/>
     <col min="2" max="8" width="42.1640625" style="1" customWidth="1"/>
     <col min="9" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="90" customHeight="1"/>
-    <row r="2" spans="1:8" ht="34">
+    <row r="1" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="2" spans="1:8" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="24">
+    <row r="3" spans="1:8" ht="24" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="70" customHeight="1">
+    <row r="4" spans="1:8" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="57" t="s">
         <v>358</v>
       </c>
       <c r="B4" s="57"/>
       <c r="C4" s="21"/>
     </row>
-    <row r="5" spans="1:8" ht="15" thickBot="1"/>
-    <row r="6" spans="1:8" ht="38.5" customHeight="1" thickBot="1">
+    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:8" ht="38.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>47</v>
       </c>
@@ -8268,7 +8293,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="38.5" customHeight="1" thickBot="1">
+    <row r="7" spans="1:8" ht="38.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
         <v>119</v>
       </c>
@@ -8294,7 +8319,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="8" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A8" s="26" t="s">
         <v>265</v>
       </c>
@@ -8306,7 +8331,7 @@
       <c r="G8" s="23"/>
       <c r="H8" s="24"/>
     </row>
-    <row r="9" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="9" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A9" s="37" t="s">
         <v>266</v>
       </c>
@@ -8318,7 +8343,7 @@
       <c r="G9" s="52"/>
       <c r="H9" s="53"/>
     </row>
-    <row r="10" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="10" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="40" t="s">
         <v>332</v>
       </c>
@@ -8344,7 +8369,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="11" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="38" t="s">
         <v>333</v>
       </c>
@@ -8370,7 +8395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="12" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
         <v>267</v>
       </c>
@@ -8396,7 +8421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="13" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
         <v>268</v>
       </c>
@@ -8422,7 +8447,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="14" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
         <v>271</v>
       </c>
@@ -8448,7 +8473,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="15" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>273</v>
       </c>
@@ -8474,7 +8499,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="16" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
         <v>274</v>
       </c>
@@ -8500,7 +8525,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="17" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A17" s="36" t="s">
         <v>275</v>
       </c>
@@ -8526,7 +8551,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="18" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A18" s="39" t="s">
         <v>276</v>
       </c>
@@ -8552,7 +8577,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="19" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A19" s="26" t="s">
         <v>277</v>
       </c>
@@ -8564,7 +8589,7 @@
       <c r="G19" s="27"/>
       <c r="H19" s="28"/>
     </row>
-    <row r="20" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="20" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A20" s="36" t="s">
         <v>278</v>
       </c>
@@ -8590,7 +8615,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="21" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A21" s="36" t="s">
         <v>279</v>
       </c>
@@ -8616,7 +8641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="22" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A22" s="36" t="s">
         <v>280</v>
       </c>
@@ -8642,7 +8667,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="23" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A23" s="36" t="s">
         <v>281</v>
       </c>
@@ -8668,7 +8693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="24" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A24" s="36" t="s">
         <v>282</v>
       </c>
@@ -8694,7 +8719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="25" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A25" s="36" t="s">
         <v>283</v>
       </c>
@@ -8720,7 +8745,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="26" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A26" s="36" t="s">
         <v>284</v>
       </c>
@@ -8746,7 +8771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="27" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A27" s="39" t="s">
         <v>285</v>
       </c>
@@ -8772,7 +8797,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="28" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A28" s="26" t="s">
         <v>286</v>
       </c>
@@ -8784,7 +8809,7 @@
       <c r="G28" s="27"/>
       <c r="H28" s="28"/>
     </row>
-    <row r="29" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="29" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A29" s="49" t="s">
         <v>287</v>
       </c>
@@ -8810,7 +8835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="30" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A30" s="36" t="s">
         <v>288</v>
       </c>
@@ -8836,7 +8861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="31" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A31" s="36" t="s">
         <v>289</v>
       </c>
@@ -8862,7 +8887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="32" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A32" s="36" t="s">
         <v>367</v>
       </c>
@@ -8888,7 +8913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="33" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A33" s="36" t="s">
         <v>290</v>
       </c>
@@ -8914,7 +8939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="34" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A34" s="39" t="s">
         <v>291</v>
       </c>
@@ -8940,7 +8965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="35" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A35" s="26" t="s">
         <v>292</v>
       </c>
@@ -8952,7 +8977,7 @@
       <c r="G35" s="27"/>
       <c r="H35" s="28"/>
     </row>
-    <row r="36" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="36" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A36" s="49" t="s">
         <v>293</v>
       </c>
@@ -8978,7 +9003,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="37" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A37" s="36" t="s">
         <v>294</v>
       </c>
@@ -9004,7 +9029,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="38" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A38" s="36" t="s">
         <v>295</v>
       </c>
@@ -9030,7 +9055,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="39" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A39" s="36" t="s">
         <v>296</v>
       </c>
@@ -9056,7 +9081,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="40" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A40" s="36" t="s">
         <v>297</v>
       </c>
@@ -9082,7 +9107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="41" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A41" s="36" t="s">
         <v>298</v>
       </c>
@@ -9108,7 +9133,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="42" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A42" s="36" t="s">
         <v>299</v>
       </c>
@@ -9134,7 +9159,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="43" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A43" s="36" t="s">
         <v>300</v>
       </c>
@@ -9160,7 +9185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="67" customHeight="1" thickBot="1">
+    <row r="44" spans="1:8" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A44" s="36" t="s">
         <v>301</v>
       </c>
@@ -9186,7 +9211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="114" customHeight="1">
+    <row r="45" spans="1:8" ht="114" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="58" t="s">
         <v>320</v>
       </c>
@@ -9209,36 +9234,36 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="73" style="1" customWidth="1"/>
     <col min="2" max="3" width="42.1640625" style="1" customWidth="1"/>
     <col min="4" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="90" customHeight="1"/>
-    <row r="2" spans="1:3" ht="34">
+    <row r="1" spans="1:3" ht="90" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="24">
+    <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="70" customHeight="1">
+    <row r="4" spans="1:3" ht="70" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="57" t="s">
         <v>359</v>
       </c>
       <c r="B4" s="57"/>
       <c r="C4" s="21"/>
     </row>
-    <row r="5" spans="1:3" ht="15" thickBot="1"/>
-    <row r="6" spans="1:3" ht="38.5" customHeight="1" thickBot="1">
+    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:3" ht="38.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>47</v>
       </c>
@@ -9246,7 +9271,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="38.5" customHeight="1" thickBot="1">
+    <row r="7" spans="1:3" ht="38.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
         <v>119</v>
       </c>
@@ -9257,21 +9282,21 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="8" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A8" s="33" t="s">
         <v>121</v>
       </c>
       <c r="B8" s="34"/>
       <c r="C8" s="35"/>
     </row>
-    <row r="9" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="9" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A9" s="37" t="s">
         <v>322</v>
       </c>
       <c r="B9" s="54"/>
       <c r="C9" s="55"/>
     </row>
-    <row r="10" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="10" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="40" t="s">
         <v>303</v>
       </c>
@@ -9282,7 +9307,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="11" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="38" t="s">
         <v>304</v>
       </c>
@@ -9293,14 +9318,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="12" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A12" s="37" t="s">
         <v>321</v>
       </c>
       <c r="B12" s="54"/>
       <c r="C12" s="55"/>
     </row>
-    <row r="13" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="13" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" s="38" t="s">
         <v>305</v>
       </c>
@@ -9311,7 +9336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="14" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A14" s="38" t="s">
         <v>306</v>
       </c>
@@ -9322,7 +9347,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="15" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>166</v>
       </c>
@@ -9333,7 +9358,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="16" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
         <v>126</v>
       </c>
@@ -9344,7 +9369,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="17" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A17" s="36" t="s">
         <v>167</v>
       </c>
@@ -9355,14 +9380,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="18" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A18" s="37" t="s">
         <v>323</v>
       </c>
       <c r="B18" s="54"/>
       <c r="C18" s="55"/>
     </row>
-    <row r="19" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="19" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A19" s="38" t="s">
         <v>168</v>
       </c>
@@ -9373,7 +9398,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="20" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A20" s="38" t="s">
         <v>169</v>
       </c>
@@ -9384,7 +9409,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="21" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A21" s="36" t="s">
         <v>170</v>
       </c>
@@ -9395,7 +9420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="22" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A22" s="36" t="s">
         <v>171</v>
       </c>
@@ -9406,7 +9431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="23" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A23" s="36" t="s">
         <v>172</v>
       </c>
@@ -9417,7 +9442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="24" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A24" s="36" t="s">
         <v>173</v>
       </c>
@@ -9428,7 +9453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="25" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A25" s="36" t="s">
         <v>174</v>
       </c>
@@ -9439,21 +9464,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="26" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A26" s="26" t="s">
         <v>175</v>
       </c>
       <c r="B26" s="27"/>
       <c r="C26" s="28"/>
     </row>
-    <row r="27" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="27" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A27" s="37" t="s">
         <v>328</v>
       </c>
       <c r="B27" s="54"/>
       <c r="C27" s="55"/>
     </row>
-    <row r="28" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="28" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A28" s="40" t="s">
         <v>307</v>
       </c>
@@ -9464,7 +9489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="29" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A29" s="38" t="s">
         <v>212</v>
       </c>
@@ -9475,7 +9500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="30" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A30" s="36" t="s">
         <v>177</v>
       </c>
@@ -9486,7 +9511,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="31" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A31" s="36" t="s">
         <v>178</v>
       </c>
@@ -9497,7 +9522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="32" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A32" s="36" t="s">
         <v>179</v>
       </c>
@@ -9508,14 +9533,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="33" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A33" s="37" t="s">
         <v>327</v>
       </c>
       <c r="B33" s="54"/>
       <c r="C33" s="55"/>
     </row>
-    <row r="34" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="34" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A34" s="38" t="s">
         <v>213</v>
       </c>
@@ -9526,7 +9551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="35" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A35" s="38" t="s">
         <v>214</v>
       </c>
@@ -9537,7 +9562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="36" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A36" s="36" t="s">
         <v>215</v>
       </c>
@@ -9548,7 +9573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="37" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A37" s="36" t="s">
         <v>181</v>
       </c>
@@ -9559,14 +9584,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="38" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A38" s="37" t="s">
         <v>326</v>
       </c>
       <c r="B38" s="54"/>
       <c r="C38" s="55"/>
     </row>
-    <row r="39" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="39" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A39" s="38" t="s">
         <v>216</v>
       </c>
@@ -9577,7 +9602,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="40" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A40" s="38" t="s">
         <v>308</v>
       </c>
@@ -9588,7 +9613,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="41" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A41" s="36" t="s">
         <v>184</v>
       </c>
@@ -9599,7 +9624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="42" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A42" s="36" t="s">
         <v>185</v>
       </c>
@@ -9610,7 +9635,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="43" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A43" s="36" t="s">
         <v>309</v>
       </c>
@@ -9621,14 +9646,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="44" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A44" s="37" t="s">
         <v>325</v>
       </c>
       <c r="B44" s="54"/>
       <c r="C44" s="55"/>
     </row>
-    <row r="45" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="45" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A45" s="38" t="s">
         <v>310</v>
       </c>
@@ -9639,7 +9664,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="46" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A46" s="51" t="s">
         <v>311</v>
       </c>
@@ -9650,7 +9675,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="47" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A47" s="39" t="s">
         <v>312</v>
       </c>
@@ -9661,14 +9686,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="48" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A48" s="26" t="s">
         <v>222</v>
       </c>
       <c r="B48" s="27"/>
       <c r="C48" s="28"/>
     </row>
-    <row r="49" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="49" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A49" s="49" t="s">
         <v>147</v>
       </c>
@@ -9679,7 +9704,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="50" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A50" s="36" t="s">
         <v>223</v>
       </c>
@@ -9690,7 +9715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="51" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A51" s="36" t="s">
         <v>194</v>
       </c>
@@ -9701,7 +9726,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="52" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A52" s="36" t="s">
         <v>365</v>
       </c>
@@ -9712,14 +9737,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="53" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A53" s="37" t="s">
         <v>324</v>
       </c>
       <c r="B53" s="54"/>
       <c r="C53" s="55"/>
     </row>
-    <row r="54" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="54" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A54" s="38" t="s">
         <v>313</v>
       </c>
@@ -9730,7 +9755,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="55" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A55" s="38" t="s">
         <v>314</v>
       </c>
@@ -9741,7 +9766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="56" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A56" s="38" t="s">
         <v>315</v>
       </c>
@@ -9752,7 +9777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="57" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A57" s="36" t="s">
         <v>224</v>
       </c>
@@ -9763,14 +9788,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="58" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A58" s="26" t="s">
         <v>198</v>
       </c>
       <c r="B58" s="27"/>
       <c r="C58" s="28"/>
     </row>
-    <row r="59" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="59" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A59" s="49" t="s">
         <v>199</v>
       </c>
@@ -9781,7 +9806,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="60" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A60" s="36" t="s">
         <v>316</v>
       </c>
@@ -9792,7 +9817,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="61" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A61" s="36" t="s">
         <v>201</v>
       </c>
@@ -9803,7 +9828,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="62" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A62" s="36" t="s">
         <v>202</v>
       </c>
@@ -9814,7 +9839,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="63" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A63" s="36" t="s">
         <v>203</v>
       </c>
@@ -9825,7 +9850,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="64" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A64" s="36" t="s">
         <v>204</v>
       </c>
@@ -9836,7 +9861,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="65" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A65" s="36" t="s">
         <v>205</v>
       </c>
@@ -9847,7 +9872,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="67" customHeight="1" thickBot="1">
+    <row r="66" spans="1:3" ht="67" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A66" s="36" t="s">
         <v>206</v>
       </c>

</xml_diff>